<commit_message>
corrected the Data Provider
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1CD3109-5578-48F2-8F0C-8B43EC93B2ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3118CA30-2887-4D61-9805-B3E3ED693821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5625" yWindow="885" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestDataSheet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t>testing@yahoo.co.in</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t>Tech Lead</t>
+  </si>
+  <si>
+    <t>validateCreateCustomerAPI</t>
   </si>
 </sst>
 </file>
@@ -121,7 +124,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -137,6 +140,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -169,7 +178,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -179,6 +188,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -460,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -510,7 +520,7 @@
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="2"/>
@@ -546,7 +556,7 @@
       <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B8" s="2"/>
@@ -602,12 +612,40 @@
       <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>